<commit_message>
doc: add 2 more entry in product backlog and complete the usecase diagram
</commit_message>
<xml_diff>
--- a/Backlog/SWP391-ProFile_Backlog.xlsx
+++ b/Backlog/SWP391-ProFile_Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Remove digital folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move physical document </t>
+  </si>
+  <si>
+    <t>Auhorization physical document</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>Authorization digital document</t>
   </si>
 </sst>
 </file>
@@ -708,10 +720,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:G38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -784,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -979,7 +991,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>5</v>
@@ -1229,15 +1241,60 @@
       <c r="F38" s="5"/>
       <c r="G38" s="10"/>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="10"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D41">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G41">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C41">
       <formula1>"Simple, Medium, Complex"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
docs: add iteration 1 items
</commit_message>
<xml_diff>
--- a/Backlog/SWP391-ProFile_Backlog.xlsx
+++ b/Backlog/SWP391-ProFile_Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentation\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentation\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753F2CAE-DEE6-41E2-A9B3-FF3BB8D25060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="1995" windowWidth="26835" windowHeight="14880"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -181,12 +182,15 @@
   </si>
   <si>
     <t>Authorization digital document</t>
+  </si>
+  <si>
+    <t>Iteration 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -326,7 +330,7 @@
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 5" xfId="2"/>
+    <cellStyle name="Normal 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -716,59 +720,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
-    <col min="8" max="228" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" customWidth="1"/>
+    <col min="8" max="228" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="19.2" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
@@ -791,7 +795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -801,12 +805,14 @@
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -821,7 +827,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -836,7 +842,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -846,12 +852,14 @@
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -866,7 +874,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -881,7 +889,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
@@ -896,7 +904,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
@@ -911,7 +919,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
@@ -926,7 +934,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
@@ -936,12 +944,14 @@
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -951,12 +961,14 @@
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -966,12 +978,14 @@
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>30</v>
       </c>
@@ -986,7 +1000,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
@@ -1001,7 +1015,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>32</v>
       </c>
@@ -1016,7 +1030,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
@@ -1031,7 +1045,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>34</v>
       </c>
@@ -1046,7 +1060,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>35</v>
       </c>
@@ -1061,7 +1075,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>36</v>
       </c>
@@ -1071,42 +1085,48 @@
       <c r="C27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>25</v>
+      <c r="B28" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>25</v>
+      <c r="B29" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>39</v>
       </c>
@@ -1116,42 +1136,48 @@
       <c r="C30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>25</v>
+      <c r="B31" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>25</v>
+      <c r="B32" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>43</v>
       </c>
@@ -1166,7 +1192,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>46</v>
       </c>
@@ -1181,7 +1207,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>42</v>
       </c>
@@ -1196,7 +1222,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>47</v>
       </c>
@@ -1211,7 +1237,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>44</v>
       </c>
@@ -1226,7 +1252,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>45</v>
       </c>
@@ -1241,7 +1267,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>48</v>
       </c>
@@ -1256,7 +1282,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>49</v>
       </c>
@@ -1266,12 +1292,14 @@
       <c r="C40" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>51</v>
       </c>
@@ -1288,13 +1316,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D41" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G41" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C41" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Simple, Medium, Complex"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
docs: add search user
</commit_message>
<xml_diff>
--- a/Backlog/SWP391-ProFile_Backlog.xlsx
+++ b/Backlog/SWP391-ProFile_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentation\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753F2CAE-DEE6-41E2-A9B3-FF3BB8D25060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D721724-4F13-474F-9DF3-11B5DB9DD84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="54">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Iteration 1</t>
+  </si>
+  <si>
+    <t>Search users</t>
   </si>
 </sst>
 </file>
@@ -724,10 +727,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -970,13 +973,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>52</v>
@@ -987,25 +990,27 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>5</v>
@@ -1017,10 +1022,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
@@ -1032,7 +1037,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>25</v>
@@ -1047,7 +1052,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>25</v>
@@ -1062,7 +1067,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>25</v>
@@ -1077,7 +1082,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>25</v>
@@ -1085,19 +1090,17 @@
       <c r="C27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="D27" s="10"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
@@ -1111,7 +1114,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>11</v>
@@ -1128,10 +1131,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>5</v>
@@ -1145,10 +1148,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -1162,7 +1165,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>11</v>
@@ -1179,22 +1182,24 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>25</v>
@@ -1209,7 +1214,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>25</v>
@@ -1224,7 +1229,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>25</v>
@@ -1239,7 +1244,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>25</v>
@@ -1253,26 +1258,26 @@
       <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="10"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
       <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>5</v>
@@ -1284,24 +1289,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>52</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D40" s="10"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>25</v>
@@ -1309,20 +1312,37 @@
       <c r="C41" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="10"/>
+      <c r="D41" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="10"/>
     </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="10"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D41" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G41" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G42" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C41" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C42" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Simple, Medium, Complex"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>